<commit_message>
Pet Supermarket each to case QTY
</commit_message>
<xml_diff>
--- a/Finished/PetSupermarket/Pet Supermarket Label Request PO 706425 11.12.2024.xlsx
+++ b/Finished/PetSupermarket/Pet Supermarket Label Request PO 706425 11.12.2024.xlsx
@@ -1048,7 +1048,11 @@
           <t>mixed</t>
         </is>
       </c>
-      <c r="F14" s="24" t="n"/>
+      <c r="F14" s="43" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
       <c r="G14" s="43" t="inlineStr">
         <is>
           <t>mixed</t>

</xml_diff>